<commit_message>
Updating hyperlinks for Contents page for final formatting. Updating helper function documentation.
</commit_message>
<xml_diff>
--- a/data/static_tables/formatting/egrid_contents_page.xlsx
+++ b/data/static_tables/formatting/egrid_contents_page.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\projects\eGrid\production_model\users\gofortht\data\static_tables\formatting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{861E6C5A-4518-4E17-9F4E-BE4BCAE3E548}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C274463-2F75-474B-9991-BE53E2AD1DE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
   <si>
     <t xml:space="preserve">Table of Contents </t>
   </si>
@@ -172,37 +172,40 @@
     <t>3) Adjustment Values (emissions, heat input, heat rate)</t>
   </si>
   <si>
+    <t>Unit year 2023 data</t>
+  </si>
+  <si>
+    <t>Generator year 2023 data</t>
+  </si>
+  <si>
+    <t>Plant year 2023 data</t>
+  </si>
+  <si>
+    <t>State year 2023 data</t>
+  </si>
+  <si>
+    <t>Balancing authority area year 2023 data</t>
+  </si>
+  <si>
+    <t>eGRID subregion year 2023 data</t>
+  </si>
+  <si>
+    <t>NERC region year 2023 data</t>
+  </si>
+  <si>
+    <t>U.S. year 2023 data</t>
+  </si>
+  <si>
+    <t>Grid Gross Loss (%) year 2023 data</t>
+  </si>
+  <si>
+    <t>Surrounding demographic data for eGRID2023 plants</t>
+  </si>
+  <si>
     <t>eGRID2023 Unit, Generator, Plant, State, Balancing Authority Area, eGRID Subregion, NERC Region, U.S., and Grid Gross Loss (%) Data Files</t>
   </si>
   <si>
     <t>eGRID2023_Data.xlsx</t>
-  </si>
-  <si>
-    <t>Unit year 2023 data</t>
-  </si>
-  <si>
-    <t>Generator year 2023 data</t>
-  </si>
-  <si>
-    <t>Plant year 2023 data</t>
-  </si>
-  <si>
-    <t>State year 2023 data</t>
-  </si>
-  <si>
-    <t>Balancing authority area year 2023 data</t>
-  </si>
-  <si>
-    <t>eGRID subregion year 2023 data</t>
-  </si>
-  <si>
-    <t>NERC region year 2023 data</t>
-  </si>
-  <si>
-    <t>U.S. year 2023 data</t>
-  </si>
-  <si>
-    <t>Grid Gross Loss (%) year 2023 data</t>
   </si>
 </sst>
 </file>
@@ -778,7 +781,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="113">
+  <cellXfs count="116">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -919,6 +922,15 @@
     <xf numFmtId="0" fontId="12" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1417,10 +1429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S53"/>
+  <dimension ref="A1:S54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="N26" sqref="N26:O26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1434,77 +1446,77 @@
     <col min="12" max="19" width="5.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="9.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:11" ht="18" x14ac:dyDescent="0.25">
-      <c r="B2" s="98" t="s">
+      <c r="B2" s="101" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="99"/>
-      <c r="D2" s="99"/>
-      <c r="E2" s="99"/>
-      <c r="F2" s="99"/>
-      <c r="G2" s="99"/>
-      <c r="H2" s="99"/>
-      <c r="I2" s="99"/>
-      <c r="J2" s="99"/>
-      <c r="K2" s="100"/>
+      <c r="C2" s="102"/>
+      <c r="D2" s="102"/>
+      <c r="E2" s="102"/>
+      <c r="F2" s="102"/>
+      <c r="G2" s="102"/>
+      <c r="H2" s="102"/>
+      <c r="I2" s="102"/>
+      <c r="J2" s="102"/>
+      <c r="K2" s="103"/>
     </row>
     <row r="3" spans="2:11" ht="18" x14ac:dyDescent="0.25">
-      <c r="B3" s="101" t="s">
+      <c r="B3" s="104" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="102"/>
-      <c r="D3" s="102"/>
-      <c r="E3" s="102"/>
-      <c r="F3" s="102"/>
-      <c r="G3" s="102"/>
-      <c r="H3" s="102"/>
-      <c r="I3" s="102"/>
-      <c r="J3" s="102"/>
-      <c r="K3" s="103"/>
+      <c r="C3" s="105"/>
+      <c r="D3" s="105"/>
+      <c r="E3" s="105"/>
+      <c r="F3" s="105"/>
+      <c r="G3" s="105"/>
+      <c r="H3" s="105"/>
+      <c r="I3" s="105"/>
+      <c r="J3" s="105"/>
+      <c r="K3" s="106"/>
     </row>
     <row r="4" spans="2:11" ht="18" x14ac:dyDescent="0.25">
-      <c r="B4" s="104" t="s">
-        <v>46</v>
-      </c>
-      <c r="C4" s="102"/>
-      <c r="D4" s="102"/>
-      <c r="E4" s="102"/>
-      <c r="F4" s="102"/>
-      <c r="G4" s="102"/>
-      <c r="H4" s="102"/>
-      <c r="I4" s="102"/>
-      <c r="J4" s="102"/>
-      <c r="K4" s="103"/>
+      <c r="B4" s="107" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" s="105"/>
+      <c r="D4" s="105"/>
+      <c r="E4" s="105"/>
+      <c r="F4" s="105"/>
+      <c r="G4" s="105"/>
+      <c r="H4" s="105"/>
+      <c r="I4" s="105"/>
+      <c r="J4" s="105"/>
+      <c r="K4" s="106"/>
     </row>
     <row r="5" spans="2:11" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="105" t="s">
-        <v>45</v>
-      </c>
-      <c r="C5" s="106"/>
-      <c r="D5" s="106"/>
-      <c r="E5" s="106"/>
-      <c r="F5" s="106"/>
-      <c r="G5" s="106"/>
-      <c r="H5" s="106"/>
-      <c r="I5" s="106"/>
-      <c r="J5" s="106"/>
-      <c r="K5" s="107"/>
+      <c r="B5" s="108" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" s="109"/>
+      <c r="D5" s="109"/>
+      <c r="E5" s="109"/>
+      <c r="F5" s="109"/>
+      <c r="G5" s="109"/>
+      <c r="H5" s="109"/>
+      <c r="I5" s="109"/>
+      <c r="J5" s="109"/>
+      <c r="K5" s="110"/>
     </row>
     <row r="6" spans="2:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="108">
+      <c r="B6" s="111">
         <f ca="1">TODAY()</f>
         <v>45642</v>
       </c>
-      <c r="C6" s="109"/>
-      <c r="D6" s="109"/>
-      <c r="E6" s="109"/>
-      <c r="F6" s="109"/>
-      <c r="G6" s="109"/>
-      <c r="H6" s="109"/>
-      <c r="I6" s="109"/>
-      <c r="J6" s="109"/>
-      <c r="K6" s="110"/>
+      <c r="C6" s="112"/>
+      <c r="D6" s="112"/>
+      <c r="E6" s="112"/>
+      <c r="F6" s="112"/>
+      <c r="G6" s="112"/>
+      <c r="H6" s="112"/>
+      <c r="I6" s="112"/>
+      <c r="J6" s="112"/>
+      <c r="K6" s="113"/>
     </row>
     <row r="7" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
@@ -1514,15 +1526,15 @@
         <v>3</v>
       </c>
       <c r="D7" s="4"/>
-      <c r="E7" s="111" t="s">
+      <c r="E7" s="114" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="111"/>
-      <c r="G7" s="111"/>
-      <c r="H7" s="111"/>
-      <c r="I7" s="111"/>
-      <c r="J7" s="111"/>
-      <c r="K7" s="112"/>
+      <c r="F7" s="114"/>
+      <c r="G7" s="114"/>
+      <c r="H7" s="114"/>
+      <c r="I7" s="114"/>
+      <c r="J7" s="114"/>
+      <c r="K7" s="115"/>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" s="5">
@@ -1530,15 +1542,15 @@
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="7"/>
-      <c r="E8" s="63" t="s">
-        <v>47</v>
-      </c>
-      <c r="F8" s="64"/>
-      <c r="G8" s="64"/>
-      <c r="H8" s="64"/>
-      <c r="I8" s="64"/>
-      <c r="J8" s="64"/>
-      <c r="K8" s="65"/>
+      <c r="E8" s="66" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" s="67"/>
+      <c r="G8" s="67"/>
+      <c r="H8" s="67"/>
+      <c r="I8" s="67"/>
+      <c r="J8" s="67"/>
+      <c r="K8" s="68"/>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B9" s="5">
@@ -1546,15 +1558,15 @@
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="7"/>
-      <c r="E9" s="63" t="s">
-        <v>48</v>
-      </c>
-      <c r="F9" s="64"/>
-      <c r="G9" s="64"/>
-      <c r="H9" s="64"/>
-      <c r="I9" s="64"/>
-      <c r="J9" s="64"/>
-      <c r="K9" s="65"/>
+      <c r="E9" s="66" t="s">
+        <v>46</v>
+      </c>
+      <c r="F9" s="67"/>
+      <c r="G9" s="67"/>
+      <c r="H9" s="67"/>
+      <c r="I9" s="67"/>
+      <c r="J9" s="67"/>
+      <c r="K9" s="68"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B10" s="5">
@@ -1562,15 +1574,15 @@
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="7"/>
-      <c r="E10" s="63" t="s">
-        <v>49</v>
-      </c>
-      <c r="F10" s="64"/>
-      <c r="G10" s="64"/>
-      <c r="H10" s="64"/>
-      <c r="I10" s="64"/>
-      <c r="J10" s="64"/>
-      <c r="K10" s="65"/>
+      <c r="E10" s="66" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" s="67"/>
+      <c r="G10" s="67"/>
+      <c r="H10" s="67"/>
+      <c r="I10" s="67"/>
+      <c r="J10" s="67"/>
+      <c r="K10" s="68"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B11" s="5">
@@ -1578,15 +1590,15 @@
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="7"/>
-      <c r="E11" s="63" t="s">
-        <v>50</v>
-      </c>
-      <c r="F11" s="64"/>
-      <c r="G11" s="64"/>
-      <c r="H11" s="64"/>
-      <c r="I11" s="64"/>
-      <c r="J11" s="64"/>
-      <c r="K11" s="65"/>
+      <c r="E11" s="66" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" s="67"/>
+      <c r="G11" s="67"/>
+      <c r="H11" s="67"/>
+      <c r="I11" s="67"/>
+      <c r="J11" s="67"/>
+      <c r="K11" s="68"/>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B12" s="5">
@@ -1594,15 +1606,15 @@
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="7"/>
-      <c r="E12" s="63" t="s">
-        <v>51</v>
-      </c>
-      <c r="F12" s="64"/>
-      <c r="G12" s="64"/>
-      <c r="H12" s="64"/>
-      <c r="I12" s="64"/>
-      <c r="J12" s="64"/>
-      <c r="K12" s="65"/>
+      <c r="E12" s="66" t="s">
+        <v>49</v>
+      </c>
+      <c r="F12" s="67"/>
+      <c r="G12" s="67"/>
+      <c r="H12" s="67"/>
+      <c r="I12" s="67"/>
+      <c r="J12" s="67"/>
+      <c r="K12" s="68"/>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B13" s="5">
@@ -1610,15 +1622,15 @@
       </c>
       <c r="C13" s="6"/>
       <c r="D13" s="7"/>
-      <c r="E13" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="F13" s="64"/>
-      <c r="G13" s="64"/>
-      <c r="H13" s="64"/>
-      <c r="I13" s="64"/>
-      <c r="J13" s="64"/>
-      <c r="K13" s="65"/>
+      <c r="E13" s="66" t="s">
+        <v>50</v>
+      </c>
+      <c r="F13" s="67"/>
+      <c r="G13" s="67"/>
+      <c r="H13" s="67"/>
+      <c r="I13" s="67"/>
+      <c r="J13" s="67"/>
+      <c r="K13" s="68"/>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B14" s="5">
@@ -1626,15 +1638,15 @@
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="7"/>
-      <c r="E14" s="63" t="s">
-        <v>53</v>
-      </c>
-      <c r="F14" s="64"/>
-      <c r="G14" s="64"/>
-      <c r="H14" s="64"/>
-      <c r="I14" s="64"/>
-      <c r="J14" s="64"/>
-      <c r="K14" s="65"/>
+      <c r="E14" s="66" t="s">
+        <v>51</v>
+      </c>
+      <c r="F14" s="67"/>
+      <c r="G14" s="67"/>
+      <c r="H14" s="67"/>
+      <c r="I14" s="67"/>
+      <c r="J14" s="67"/>
+      <c r="K14" s="68"/>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" s="5">
@@ -1642,15 +1654,15 @@
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="7"/>
-      <c r="E15" s="63" t="s">
-        <v>54</v>
-      </c>
-      <c r="F15" s="64"/>
-      <c r="G15" s="64"/>
-      <c r="H15" s="64"/>
-      <c r="I15" s="64"/>
-      <c r="J15" s="64"/>
-      <c r="K15" s="65"/>
+      <c r="E15" s="66" t="s">
+        <v>52</v>
+      </c>
+      <c r="F15" s="67"/>
+      <c r="G15" s="67"/>
+      <c r="H15" s="67"/>
+      <c r="I15" s="67"/>
+      <c r="J15" s="67"/>
+      <c r="K15" s="68"/>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B16" s="5">
@@ -1658,58 +1670,59 @@
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="7"/>
-      <c r="E16" s="63" t="s">
-        <v>55</v>
-      </c>
-      <c r="F16" s="64"/>
-      <c r="G16" s="64"/>
-      <c r="H16" s="64"/>
-      <c r="I16" s="64"/>
-      <c r="J16" s="64"/>
-      <c r="K16" s="65"/>
-    </row>
-    <row r="17" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="8"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
-      <c r="J17" s="12"/>
-      <c r="K17" s="13"/>
+      <c r="E16" s="66" t="s">
+        <v>53</v>
+      </c>
+      <c r="F16" s="67"/>
+      <c r="G16" s="67"/>
+      <c r="H16" s="67"/>
+      <c r="I16" s="67"/>
+      <c r="J16" s="67"/>
+      <c r="K16" s="68"/>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B17" s="5">
+        <v>10</v>
+      </c>
+      <c r="C17" s="6"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="57" t="s">
+        <v>54</v>
+      </c>
+      <c r="F17" s="58"/>
+      <c r="G17" s="58"/>
+      <c r="H17" s="58"/>
+      <c r="I17" s="58"/>
+      <c r="J17" s="58"/>
+      <c r="K17" s="59"/>
     </row>
     <row r="18" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="14"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="14"/>
-      <c r="K18" s="14"/>
-    </row>
-    <row r="19" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B19" s="78" t="s">
+      <c r="B18" s="8"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="12"/>
+      <c r="K18" s="13"/>
+    </row>
+    <row r="19" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="14"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="14"/>
+    </row>
+    <row r="20" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B20" s="81" t="s">
         <v>5</v>
-      </c>
-      <c r="C19" s="79"/>
-      <c r="D19" s="79"/>
-      <c r="E19" s="79"/>
-      <c r="F19" s="79"/>
-      <c r="G19" s="79"/>
-      <c r="H19" s="79"/>
-      <c r="I19" s="79"/>
-      <c r="J19" s="79"/>
-      <c r="K19" s="80"/>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A20" s="17"/>
-      <c r="B20" s="81" t="s">
-        <v>6</v>
       </c>
       <c r="C20" s="82"/>
       <c r="D20" s="82"/>
@@ -1721,10 +1734,10 @@
       <c r="J20" s="82"/>
       <c r="K20" s="83"/>
     </row>
-    <row r="21" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="17"/>
       <c r="B21" s="84" t="s">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="C21" s="85"/>
       <c r="D21" s="85"/>
@@ -1736,121 +1749,114 @@
       <c r="J21" s="85"/>
       <c r="K21" s="86"/>
     </row>
-    <row r="22" spans="1:19" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="18"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
-      <c r="H22" s="18"/>
-      <c r="I22" s="18"/>
-      <c r="J22" s="18"/>
-      <c r="K22" s="18"/>
-    </row>
-    <row r="23" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B23" s="87" t="s">
+    <row r="22" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="17"/>
+      <c r="B22" s="87" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" s="88"/>
+      <c r="D22" s="88"/>
+      <c r="E22" s="88"/>
+      <c r="F22" s="88"/>
+      <c r="G22" s="88"/>
+      <c r="H22" s="88"/>
+      <c r="I22" s="88"/>
+      <c r="J22" s="88"/>
+      <c r="K22" s="89"/>
+    </row>
+    <row r="23" spans="1:19" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="18"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="18"/>
+      <c r="I23" s="18"/>
+      <c r="J23" s="18"/>
+      <c r="K23" s="18"/>
+    </row>
+    <row r="24" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B24" s="90" t="s">
         <v>7</v>
       </c>
-      <c r="C23" s="88"/>
-      <c r="D23" s="88"/>
-      <c r="E23" s="88"/>
-      <c r="F23" s="88"/>
-      <c r="G23" s="88"/>
-      <c r="H23" s="88"/>
-      <c r="I23" s="88"/>
-      <c r="J23" s="88"/>
-      <c r="K23" s="88"/>
-      <c r="L23" s="88"/>
-      <c r="M23" s="88"/>
-      <c r="N23" s="88"/>
-      <c r="O23" s="88"/>
-      <c r="P23" s="88"/>
-      <c r="Q23" s="89"/>
-      <c r="R23"/>
-      <c r="S23"/>
-    </row>
-    <row r="24" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="C24" s="20"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="20"/>
-      <c r="G24" s="20"/>
-      <c r="H24" s="20"/>
-      <c r="I24" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="J24" s="90" t="s">
-        <v>10</v>
-      </c>
-      <c r="K24" s="90"/>
-      <c r="L24" s="90"/>
-      <c r="M24" s="90"/>
-      <c r="N24" s="90"/>
-      <c r="O24" s="90"/>
-      <c r="P24" s="90"/>
-      <c r="Q24" s="91"/>
+      <c r="C24" s="91"/>
+      <c r="D24" s="91"/>
+      <c r="E24" s="91"/>
+      <c r="F24" s="91"/>
+      <c r="G24" s="91"/>
+      <c r="H24" s="91"/>
+      <c r="I24" s="91"/>
+      <c r="J24" s="91"/>
+      <c r="K24" s="91"/>
+      <c r="L24" s="91"/>
+      <c r="M24" s="91"/>
+      <c r="N24" s="91"/>
+      <c r="O24" s="91"/>
+      <c r="P24" s="91"/>
+      <c r="Q24" s="92"/>
       <c r="R24"/>
       <c r="S24"/>
     </row>
-    <row r="25" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="92" t="s">
-        <v>11</v>
-      </c>
-      <c r="C25" s="93"/>
-      <c r="D25" s="93"/>
-      <c r="E25" s="93"/>
-      <c r="F25" s="93"/>
-      <c r="G25" s="93"/>
-      <c r="H25" s="94"/>
-      <c r="I25" s="22"/>
-      <c r="J25" s="23"/>
-      <c r="K25" s="23"/>
-      <c r="L25" s="23"/>
-      <c r="M25" s="23"/>
-      <c r="N25" s="23"/>
-      <c r="O25" s="23"/>
-      <c r="P25" s="23"/>
-      <c r="Q25" s="24"/>
+    <row r="25" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="J25" s="93" t="s">
+        <v>10</v>
+      </c>
+      <c r="K25" s="93"/>
+      <c r="L25" s="93"/>
+      <c r="M25" s="93"/>
+      <c r="N25" s="93"/>
+      <c r="O25" s="93"/>
+      <c r="P25" s="93"/>
+      <c r="Q25" s="94"/>
       <c r="R25"/>
       <c r="S25"/>
     </row>
     <row r="26" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="69" t="s">
-        <v>12</v>
-      </c>
-      <c r="C26" s="70"/>
-      <c r="D26" s="70"/>
-      <c r="E26" s="70"/>
-      <c r="F26" s="70"/>
-      <c r="G26" s="70"/>
-      <c r="H26" s="71"/>
-      <c r="I26" s="25"/>
-      <c r="J26" s="26"/>
-      <c r="K26" s="27"/>
-      <c r="L26" s="26"/>
-      <c r="M26" s="26"/>
-      <c r="N26" s="28"/>
-      <c r="O26" s="27"/>
-      <c r="P26" s="26"/>
-      <c r="Q26" s="29"/>
+      <c r="B26" s="95" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" s="96"/>
+      <c r="D26" s="96"/>
+      <c r="E26" s="96"/>
+      <c r="F26" s="96"/>
+      <c r="G26" s="96"/>
+      <c r="H26" s="97"/>
+      <c r="I26" s="22"/>
+      <c r="J26" s="23"/>
+      <c r="K26" s="23"/>
+      <c r="L26" s="23"/>
+      <c r="M26" s="23"/>
+      <c r="N26" s="23"/>
+      <c r="O26" s="23"/>
+      <c r="P26" s="23"/>
+      <c r="Q26" s="24"/>
       <c r="R26"/>
       <c r="S26"/>
     </row>
     <row r="27" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="95" t="s">
-        <v>44</v>
-      </c>
-      <c r="C27" s="96"/>
-      <c r="D27" s="96"/>
-      <c r="E27" s="96"/>
-      <c r="F27" s="96"/>
-      <c r="G27" s="96"/>
-      <c r="H27" s="97"/>
-      <c r="I27" s="56"/>
+      <c r="B27" s="72" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27" s="73"/>
+      <c r="D27" s="73"/>
+      <c r="E27" s="73"/>
+      <c r="F27" s="73"/>
+      <c r="G27" s="73"/>
+      <c r="H27" s="74"/>
+      <c r="I27" s="25"/>
       <c r="J27" s="26"/>
       <c r="K27" s="27"/>
       <c r="L27" s="26"/>
@@ -1863,38 +1869,38 @@
       <c r="S27"/>
     </row>
     <row r="28" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="75" t="s">
-        <v>16</v>
-      </c>
-      <c r="C28" s="76"/>
-      <c r="D28" s="76"/>
-      <c r="E28" s="76"/>
-      <c r="F28" s="76"/>
-      <c r="G28" s="76"/>
-      <c r="H28" s="77"/>
-      <c r="I28" s="30"/>
+      <c r="B28" s="98" t="s">
+        <v>44</v>
+      </c>
+      <c r="C28" s="99"/>
+      <c r="D28" s="99"/>
+      <c r="E28" s="99"/>
+      <c r="F28" s="99"/>
+      <c r="G28" s="99"/>
+      <c r="H28" s="100"/>
+      <c r="I28" s="56"/>
       <c r="J28" s="26"/>
       <c r="K28" s="27"/>
       <c r="L28" s="26"/>
       <c r="M28" s="26"/>
-      <c r="N28" s="26"/>
-      <c r="O28" s="26"/>
+      <c r="N28" s="28"/>
+      <c r="O28" s="27"/>
       <c r="P28" s="26"/>
       <c r="Q28" s="29"/>
       <c r="R28"/>
       <c r="S28"/>
     </row>
     <row r="29" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="75" t="s">
-        <v>17</v>
-      </c>
-      <c r="C29" s="76"/>
-      <c r="D29" s="76"/>
-      <c r="E29" s="76"/>
-      <c r="F29" s="76"/>
-      <c r="G29" s="76"/>
-      <c r="H29" s="77"/>
-      <c r="I29" s="31"/>
+      <c r="B29" s="78" t="s">
+        <v>16</v>
+      </c>
+      <c r="C29" s="79"/>
+      <c r="D29" s="79"/>
+      <c r="E29" s="79"/>
+      <c r="F29" s="79"/>
+      <c r="G29" s="79"/>
+      <c r="H29" s="80"/>
+      <c r="I29" s="30"/>
       <c r="J29" s="26"/>
       <c r="K29" s="27"/>
       <c r="L29" s="26"/>
@@ -1907,16 +1913,16 @@
       <c r="S29"/>
     </row>
     <row r="30" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="69" t="s">
-        <v>18</v>
-      </c>
-      <c r="C30" s="70"/>
-      <c r="D30" s="70"/>
-      <c r="E30" s="70"/>
-      <c r="F30" s="70"/>
-      <c r="G30" s="70"/>
-      <c r="H30" s="71"/>
-      <c r="I30" s="32"/>
+      <c r="B30" s="78" t="s">
+        <v>17</v>
+      </c>
+      <c r="C30" s="79"/>
+      <c r="D30" s="79"/>
+      <c r="E30" s="79"/>
+      <c r="F30" s="79"/>
+      <c r="G30" s="79"/>
+      <c r="H30" s="80"/>
+      <c r="I30" s="31"/>
       <c r="J30" s="26"/>
       <c r="K30" s="27"/>
       <c r="L30" s="26"/>
@@ -1929,16 +1935,16 @@
       <c r="S30"/>
     </row>
     <row r="31" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="69" t="s">
-        <v>19</v>
-      </c>
-      <c r="C31" s="70"/>
-      <c r="D31" s="70"/>
-      <c r="E31" s="70"/>
-      <c r="F31" s="70"/>
-      <c r="G31" s="70"/>
-      <c r="H31" s="71"/>
-      <c r="I31" s="33"/>
+      <c r="B31" s="72" t="s">
+        <v>18</v>
+      </c>
+      <c r="C31" s="73"/>
+      <c r="D31" s="73"/>
+      <c r="E31" s="73"/>
+      <c r="F31" s="73"/>
+      <c r="G31" s="73"/>
+      <c r="H31" s="74"/>
+      <c r="I31" s="32"/>
       <c r="J31" s="26"/>
       <c r="K31" s="27"/>
       <c r="L31" s="26"/>
@@ -1951,16 +1957,16 @@
       <c r="S31"/>
     </row>
     <row r="32" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="69" t="s">
-        <v>20</v>
-      </c>
-      <c r="C32" s="70"/>
-      <c r="D32" s="70"/>
-      <c r="E32" s="70"/>
-      <c r="F32" s="70"/>
-      <c r="G32" s="70"/>
-      <c r="H32" s="71"/>
-      <c r="I32" s="34"/>
+      <c r="B32" s="72" t="s">
+        <v>19</v>
+      </c>
+      <c r="C32" s="73"/>
+      <c r="D32" s="73"/>
+      <c r="E32" s="73"/>
+      <c r="F32" s="73"/>
+      <c r="G32" s="73"/>
+      <c r="H32" s="74"/>
+      <c r="I32" s="33"/>
       <c r="J32" s="26"/>
       <c r="K32" s="27"/>
       <c r="L32" s="26"/>
@@ -1974,7 +1980,7 @@
     </row>
     <row r="33" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="72" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C33" s="73"/>
       <c r="D33" s="73"/>
@@ -1982,7 +1988,7 @@
       <c r="F33" s="73"/>
       <c r="G33" s="73"/>
       <c r="H33" s="74"/>
-      <c r="I33" s="35"/>
+      <c r="I33" s="34"/>
       <c r="J33" s="26"/>
       <c r="K33" s="27"/>
       <c r="L33" s="26"/>
@@ -1995,16 +2001,16 @@
       <c r="S33"/>
     </row>
     <row r="34" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="72" t="s">
-        <v>22</v>
-      </c>
-      <c r="C34" s="73"/>
-      <c r="D34" s="73"/>
-      <c r="E34" s="73"/>
-      <c r="F34" s="73"/>
-      <c r="G34" s="73"/>
-      <c r="H34" s="74"/>
-      <c r="I34" s="36"/>
+      <c r="B34" s="75" t="s">
+        <v>21</v>
+      </c>
+      <c r="C34" s="76"/>
+      <c r="D34" s="76"/>
+      <c r="E34" s="76"/>
+      <c r="F34" s="76"/>
+      <c r="G34" s="76"/>
+      <c r="H34" s="77"/>
+      <c r="I34" s="35"/>
       <c r="J34" s="26"/>
       <c r="K34" s="27"/>
       <c r="L34" s="26"/>
@@ -2017,16 +2023,16 @@
       <c r="S34"/>
     </row>
     <row r="35" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="69" t="s">
-        <v>23</v>
-      </c>
-      <c r="C35" s="70"/>
-      <c r="D35" s="70"/>
-      <c r="E35" s="70"/>
-      <c r="F35" s="70"/>
-      <c r="G35" s="70"/>
-      <c r="H35" s="71"/>
-      <c r="I35" s="37"/>
+      <c r="B35" s="75" t="s">
+        <v>22</v>
+      </c>
+      <c r="C35" s="76"/>
+      <c r="D35" s="76"/>
+      <c r="E35" s="76"/>
+      <c r="F35" s="76"/>
+      <c r="G35" s="76"/>
+      <c r="H35" s="77"/>
+      <c r="I35" s="36"/>
       <c r="J35" s="26"/>
       <c r="K35" s="27"/>
       <c r="L35" s="26"/>
@@ -2040,7 +2046,7 @@
     </row>
     <row r="36" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="72" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C36" s="73"/>
       <c r="D36" s="73"/>
@@ -2048,7 +2054,7 @@
       <c r="F36" s="73"/>
       <c r="G36" s="73"/>
       <c r="H36" s="74"/>
-      <c r="I36" s="38"/>
+      <c r="I36" s="37"/>
       <c r="J36" s="26"/>
       <c r="K36" s="27"/>
       <c r="L36" s="26"/>
@@ -2061,16 +2067,16 @@
       <c r="S36"/>
     </row>
     <row r="37" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="72" t="s">
-        <v>25</v>
-      </c>
-      <c r="C37" s="73"/>
-      <c r="D37" s="73"/>
-      <c r="E37" s="73"/>
-      <c r="F37" s="73"/>
-      <c r="G37" s="73"/>
-      <c r="H37" s="74"/>
-      <c r="I37" s="39"/>
+      <c r="B37" s="75" t="s">
+        <v>24</v>
+      </c>
+      <c r="C37" s="76"/>
+      <c r="D37" s="76"/>
+      <c r="E37" s="76"/>
+      <c r="F37" s="76"/>
+      <c r="G37" s="76"/>
+      <c r="H37" s="77"/>
+      <c r="I37" s="38"/>
       <c r="J37" s="26"/>
       <c r="K37" s="27"/>
       <c r="L37" s="26"/>
@@ -2083,16 +2089,16 @@
       <c r="S37"/>
     </row>
     <row r="38" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="72" t="s">
-        <v>26</v>
-      </c>
-      <c r="C38" s="73"/>
-      <c r="D38" s="73"/>
-      <c r="E38" s="73"/>
-      <c r="F38" s="73"/>
-      <c r="G38" s="73"/>
-      <c r="H38" s="74"/>
-      <c r="I38" s="40"/>
+      <c r="B38" s="75" t="s">
+        <v>25</v>
+      </c>
+      <c r="C38" s="76"/>
+      <c r="D38" s="76"/>
+      <c r="E38" s="76"/>
+      <c r="F38" s="76"/>
+      <c r="G38" s="76"/>
+      <c r="H38" s="77"/>
+      <c r="I38" s="39"/>
       <c r="J38" s="26"/>
       <c r="K38" s="27"/>
       <c r="L38" s="26"/>
@@ -2105,16 +2111,16 @@
       <c r="S38"/>
     </row>
     <row r="39" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="72" t="s">
-        <v>27</v>
-      </c>
-      <c r="C39" s="73"/>
-      <c r="D39" s="73"/>
-      <c r="E39" s="73"/>
-      <c r="F39" s="73"/>
-      <c r="G39" s="73"/>
-      <c r="H39" s="74"/>
-      <c r="I39" s="41"/>
+      <c r="B39" s="75" t="s">
+        <v>26</v>
+      </c>
+      <c r="C39" s="76"/>
+      <c r="D39" s="76"/>
+      <c r="E39" s="76"/>
+      <c r="F39" s="76"/>
+      <c r="G39" s="76"/>
+      <c r="H39" s="77"/>
+      <c r="I39" s="40"/>
       <c r="J39" s="26"/>
       <c r="K39" s="27"/>
       <c r="L39" s="26"/>
@@ -2127,16 +2133,16 @@
       <c r="S39"/>
     </row>
     <row r="40" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="72" t="s">
-        <v>28</v>
-      </c>
-      <c r="C40" s="73"/>
-      <c r="D40" s="73"/>
-      <c r="E40" s="73"/>
-      <c r="F40" s="73"/>
-      <c r="G40" s="73"/>
-      <c r="H40" s="74"/>
-      <c r="I40" s="42"/>
+      <c r="B40" s="75" t="s">
+        <v>27</v>
+      </c>
+      <c r="C40" s="76"/>
+      <c r="D40" s="76"/>
+      <c r="E40" s="76"/>
+      <c r="F40" s="76"/>
+      <c r="G40" s="76"/>
+      <c r="H40" s="77"/>
+      <c r="I40" s="41"/>
       <c r="J40" s="26"/>
       <c r="K40" s="27"/>
       <c r="L40" s="26"/>
@@ -2148,132 +2154,154 @@
       <c r="R40"/>
       <c r="S40"/>
     </row>
-    <row r="41" spans="2:19" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="66" t="s">
-        <v>29</v>
-      </c>
-      <c r="C41" s="67"/>
-      <c r="D41" s="67"/>
-      <c r="E41" s="67"/>
-      <c r="F41" s="67"/>
-      <c r="G41" s="67"/>
-      <c r="H41" s="68"/>
-      <c r="I41" s="43"/>
-      <c r="J41" s="44"/>
-      <c r="K41" s="45"/>
-      <c r="L41" s="44"/>
-      <c r="M41" s="44"/>
-      <c r="N41" s="44"/>
-      <c r="O41" s="44"/>
-      <c r="P41" s="44"/>
-      <c r="Q41" s="44"/>
+    <row r="41" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="75" t="s">
+        <v>28</v>
+      </c>
+      <c r="C41" s="76"/>
+      <c r="D41" s="76"/>
+      <c r="E41" s="76"/>
+      <c r="F41" s="76"/>
+      <c r="G41" s="76"/>
+      <c r="H41" s="77"/>
+      <c r="I41" s="42"/>
+      <c r="J41" s="26"/>
+      <c r="K41" s="27"/>
+      <c r="L41" s="26"/>
+      <c r="M41" s="26"/>
+      <c r="N41" s="26"/>
+      <c r="O41" s="26"/>
+      <c r="P41" s="26"/>
+      <c r="Q41" s="29"/>
       <c r="R41"/>
       <c r="S41"/>
     </row>
-    <row r="42" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="46"/>
-      <c r="C42" s="46"/>
-      <c r="D42" s="46"/>
-      <c r="E42" s="46"/>
-      <c r="F42" s="46"/>
-      <c r="G42" s="46"/>
-      <c r="H42" s="46"/>
-      <c r="I42" s="46"/>
-      <c r="J42" s="46"/>
-      <c r="K42" s="46"/>
-    </row>
-    <row r="43" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B43" s="47" t="s">
+    <row r="42" spans="2:19" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B42" s="69" t="s">
+        <v>29</v>
+      </c>
+      <c r="C42" s="70"/>
+      <c r="D42" s="70"/>
+      <c r="E42" s="70"/>
+      <c r="F42" s="70"/>
+      <c r="G42" s="70"/>
+      <c r="H42" s="71"/>
+      <c r="I42" s="43"/>
+      <c r="J42" s="44"/>
+      <c r="K42" s="45"/>
+      <c r="L42" s="44"/>
+      <c r="M42" s="44"/>
+      <c r="N42" s="44"/>
+      <c r="O42" s="44"/>
+      <c r="P42" s="44"/>
+      <c r="Q42" s="44"/>
+      <c r="R42"/>
+      <c r="S42"/>
+    </row>
+    <row r="43" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B43" s="46"/>
+      <c r="C43" s="46"/>
+      <c r="D43" s="46"/>
+      <c r="E43" s="46"/>
+      <c r="F43" s="46"/>
+      <c r="G43" s="46"/>
+      <c r="H43" s="46"/>
+      <c r="I43" s="46"/>
+      <c r="J43" s="46"/>
+      <c r="K43" s="46"/>
+    </row>
+    <row r="44" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B44" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="C43" s="48"/>
-      <c r="D43" s="48"/>
-      <c r="E43" s="49"/>
-    </row>
-    <row r="44" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B44" s="50" t="s">
+      <c r="C44" s="48"/>
+      <c r="D44" s="48"/>
+      <c r="E44" s="49"/>
+    </row>
+    <row r="45" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B45" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="C44" s="51"/>
-      <c r="D44" s="51"/>
-      <c r="E44" s="52"/>
-    </row>
-    <row r="45" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="53" t="s">
+      <c r="C45" s="51"/>
+      <c r="D45" s="51"/>
+      <c r="E45" s="52"/>
+    </row>
+    <row r="46" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B46" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="C45" s="54"/>
-      <c r="D45" s="54"/>
-      <c r="E45" s="55"/>
-    </row>
-    <row r="46" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="47" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B47" s="47" t="s">
+      <c r="C46" s="54"/>
+      <c r="D46" s="54"/>
+      <c r="E46" s="55"/>
+    </row>
+    <row r="47" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="48" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B48" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="C47" s="48"/>
-      <c r="D47" s="48"/>
-      <c r="E47" s="49"/>
-    </row>
-    <row r="48" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B48" s="57" t="s">
+      <c r="C48" s="48"/>
+      <c r="D48" s="48"/>
+      <c r="E48" s="49"/>
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B49" s="60" t="s">
         <v>40</v>
       </c>
-      <c r="C48" s="58"/>
-      <c r="D48" s="58" t="s">
+      <c r="C49" s="61"/>
+      <c r="D49" s="61" t="s">
         <v>41</v>
       </c>
-      <c r="E48" s="61"/>
-    </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B49" s="57" t="s">
+      <c r="E49" s="64"/>
+    </row>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B50" s="60" t="s">
         <v>37</v>
       </c>
-      <c r="C49" s="58"/>
-      <c r="D49" s="58" t="s">
+      <c r="C50" s="61"/>
+      <c r="D50" s="61" t="s">
         <v>38</v>
       </c>
-      <c r="E49" s="61"/>
-    </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B50" s="57" t="s">
+      <c r="E50" s="64"/>
+    </row>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B51" s="60" t="s">
         <v>32</v>
       </c>
-      <c r="C50" s="58"/>
-      <c r="D50" s="58" t="s">
+      <c r="C51" s="61"/>
+      <c r="D51" s="61" t="s">
         <v>33</v>
       </c>
-      <c r="E50" s="61"/>
-    </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B51" s="57" t="s">
+      <c r="E51" s="64"/>
+    </row>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B52" s="60" t="s">
         <v>39</v>
       </c>
-      <c r="C51" s="58"/>
-      <c r="D51" s="58" t="s">
+      <c r="C52" s="61"/>
+      <c r="D52" s="61" t="s">
         <v>34</v>
       </c>
-      <c r="E51" s="61"/>
-    </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B52" s="57" t="s">
+      <c r="E52" s="64"/>
+    </row>
+    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B53" s="60" t="s">
         <v>36</v>
       </c>
-      <c r="C52" s="58"/>
-      <c r="D52" s="58" t="s">
+      <c r="C53" s="61"/>
+      <c r="D53" s="61" t="s">
         <v>35</v>
       </c>
-      <c r="E52" s="61"/>
-    </row>
-    <row r="53" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="59" t="s">
+      <c r="E53" s="64"/>
+    </row>
+    <row r="54" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B54" s="62" t="s">
         <v>42</v>
       </c>
-      <c r="C53" s="60"/>
-      <c r="D53" s="60" t="s">
+      <c r="C54" s="63"/>
+      <c r="D54" s="63" t="s">
         <v>43</v>
       </c>
-      <c r="E53" s="62"/>
+      <c r="E54" s="65"/>
     </row>
   </sheetData>
   <mergeCells count="49">
@@ -2289,24 +2317,23 @@
     <mergeCell ref="E10:K10"/>
     <mergeCell ref="E11:K11"/>
     <mergeCell ref="E12:K12"/>
-    <mergeCell ref="B40:H40"/>
-    <mergeCell ref="B29:H29"/>
-    <mergeCell ref="B19:K19"/>
+    <mergeCell ref="B41:H41"/>
+    <mergeCell ref="B30:H30"/>
     <mergeCell ref="B20:K20"/>
     <mergeCell ref="B21:K21"/>
-    <mergeCell ref="B23:Q23"/>
-    <mergeCell ref="J24:Q24"/>
-    <mergeCell ref="B25:H25"/>
+    <mergeCell ref="B22:K22"/>
+    <mergeCell ref="B24:Q24"/>
+    <mergeCell ref="J25:Q25"/>
     <mergeCell ref="B26:H26"/>
+    <mergeCell ref="B27:H27"/>
+    <mergeCell ref="B29:H29"/>
     <mergeCell ref="B28:H28"/>
-    <mergeCell ref="B27:H27"/>
     <mergeCell ref="E16:K16"/>
     <mergeCell ref="E15:K15"/>
     <mergeCell ref="E14:K14"/>
-    <mergeCell ref="B48:C48"/>
     <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B41:H41"/>
-    <mergeCell ref="B30:H30"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B42:H42"/>
     <mergeCell ref="B31:H31"/>
     <mergeCell ref="B32:H32"/>
     <mergeCell ref="B33:H33"/>
@@ -2316,20 +2343,21 @@
     <mergeCell ref="B37:H37"/>
     <mergeCell ref="B38:H38"/>
     <mergeCell ref="B39:H39"/>
-    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B40:H40"/>
     <mergeCell ref="B51:C51"/>
     <mergeCell ref="B52:C52"/>
     <mergeCell ref="B53:C53"/>
-    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="B54:C54"/>
     <mergeCell ref="D49:E49"/>
     <mergeCell ref="D50:E50"/>
     <mergeCell ref="D51:E51"/>
     <mergeCell ref="D52:E52"/>
     <mergeCell ref="D53:E53"/>
+    <mergeCell ref="D54:E54"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B20:K20" r:id="rId1" display="Customer Satisfaction Survey" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="B21:K21" r:id="rId2" display="Contact EPA" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="B21:K21" r:id="rId1" display="Customer Satisfaction Survey" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="B22:K22" r:id="rId2" display="Contact EPA" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>

</xml_diff>